<commit_message>
Signed Ints added to xl
</commit_message>
<xml_diff>
--- a/useful references/Hex_Decimal_Binary Conversion.xlsx
+++ b/useful references/Hex_Decimal_Binary Conversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\useful references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D3A335-C573-4D5E-B810-409E5A19ADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9A7B1A-67BD-4F89-9F1C-6C704B20E98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9E27DF17-1687-49C3-9253-CE9DE59247CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>HEX</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECIMAL </t>
+  </si>
+  <si>
+    <t>U_BINARY (up to +255)</t>
+  </si>
+  <si>
+    <t>S_BINARY (-128 to +127)</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +257,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -584,21 +596,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF927923-D9B4-4DFE-AF4D-4C05DEA31251}">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.8984375" customWidth="1"/>
-    <col min="3" max="3" width="15.09765625" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.19921875" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -609,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -622,8 +635,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
@@ -634,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -647,8 +660,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>1</v>
       </c>
@@ -659,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>1111</v>
       </c>
@@ -671,6 +684,32 @@
         <f>BIN2HEX(B11)</f>
         <v>F</v>
       </c>
+    </row>
+    <row r="13" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>86</v>
+      </c>
+      <c r="C15" s="12" t="str">
+        <f>DEC2BIN(B15,8)</f>
+        <v>01010110</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>_xlfn.BASE(MOD((B15*-1), 2^8), 2, 8)</f>
+        <v>10101010</v>
+      </c>
+      <c r="E15" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>